<commit_message>
Changed files AddTest, Login Test, Project.Properties, ordering suite.xlsx
</commit_message>
<xml_diff>
--- a/webdriver_rediff/OrderingSuite.xlsx
+++ b/webdriver_rediff/OrderingSuite.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12525" windowHeight="8820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -152,7 +153,7 @@
     <t>PurchaseDate</t>
   </si>
   <si>
-    <t>25/5/2016</t>
+    <t>26/5/2016</t>
   </si>
 </sst>
 </file>
@@ -607,7 +608,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
create change order long distance test case
</commit_message>
<xml_diff>
--- a/webdriver_rediff/OrderingSuite.xlsx
+++ b/webdriver_rediff/OrderingSuite.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="18030" windowHeight="10185" activeTab="1"/>
@@ -10,12 +10,12 @@
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
   <si>
     <t>TestCases</t>
   </si>
@@ -176,7 +176,22 @@
     <t>67369192</t>
   </si>
   <si>
-    <t>26/01/2017</t>
+    <t>ChangeLongDistanceTest</t>
+  </si>
+  <si>
+    <t>TesterGirish</t>
+  </si>
+  <si>
+    <t>ServiceId</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>9560896677</t>
+  </si>
+  <si>
+    <t>16/02/2017</t>
   </si>
 </sst>
 </file>
@@ -269,15 +284,16 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -573,15 +589,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -631,6 +647,14 @@
       </c>
       <c r="B6" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -641,15 +665,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" customWidth="1"/>
@@ -692,7 +716,7 @@
       <c r="D3" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>49</v>
       </c>
     </row>
@@ -706,7 +730,7 @@
       <c r="D4" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>50</v>
       </c>
     </row>
@@ -791,7 +815,7 @@
       <c r="G14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -802,10 +826,10 @@
       <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>52</v>
       </c>
       <c r="F15" t="s">
@@ -851,30 +875,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="F21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
     <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" t="s">
-        <v>23</v>
-      </c>
-      <c r="H22" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
@@ -892,14 +896,14 @@
       <c r="E23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" t="s">
-        <v>26</v>
-      </c>
-      <c r="H23" t="s">
-        <v>29</v>
+      <c r="F23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -916,13 +920,13 @@
         <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G24" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -938,6 +942,15 @@
       <c r="E25" t="s">
         <v>15</v>
       </c>
+      <c r="F25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
@@ -952,10 +965,77 @@
       <c r="E26" t="s">
         <v>18</v>
       </c>
+      <c r="F26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" t="s">
+        <v>54</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H15" r:id="rId1"/>
+    <hyperlink ref="H30" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated properties file and developed script move order private line
</commit_message>
<xml_diff>
--- a/webdriver_rediff/OrderingSuite.xlsx
+++ b/webdriver_rediff/OrderingSuite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="18030" windowHeight="10185"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="18030" windowHeight="10185" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="63">
   <si>
     <t>TestCases</t>
   </si>
@@ -192,6 +192,18 @@
   </si>
   <si>
     <t>16/02/2017</t>
+  </si>
+  <si>
+    <t>MovePrivateLineTest</t>
+  </si>
+  <si>
+    <t>Current Service Address</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>New Service Address</t>
   </si>
 </sst>
 </file>
@@ -284,7 +296,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -294,6 +306,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -589,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -657,6 +670,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -665,10 +686,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="F22" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -681,6 +702,8 @@
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1032,11 +1055,82 @@
         <v>44</v>
       </c>
     </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34" t="s">
+        <v>54</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I34" t="s">
+        <v>61</v>
+      </c>
+      <c r="J34" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H15" r:id="rId1"/>
     <hyperlink ref="H30" r:id="rId2"/>
+    <hyperlink ref="H34" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>